<commit_message>
moved the requirements.txt to root directory
</commit_message>
<xml_diff>
--- a/data/games.xlsx
+++ b/data/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/590cc5b1e80d3c15/Documents/Projects/Game Logger Doc/game-logger/game-logger/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2E71B46853083291B0C80DD04B5ED87656CC5167" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06D21DCB-D748-4E89-BC7D-2DC95B1BE46A}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_08A957745358B3DAE0CA1CD04B5ED87656CCB19F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C5B7696-69B6-4BD9-A139-C28CB42020F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,6 +788,9 @@
     <t>ALAN WAKE 2</t>
   </si>
   <si>
+    <t>Like a Dragon Gaiden: The Man Who Erased His Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEKIRO : SHADOWS DIE TWICE </t>
   </si>
   <si>
@@ -809,6 +812,9 @@
     <t>Motive Studio</t>
   </si>
   <si>
+    <t>Like a Dragon: Infinite Wealth</t>
+  </si>
+  <si>
     <t>CALL OF DUTY BLACK OPS 6</t>
   </si>
   <si>
@@ -858,12 +864,6 @@
   </si>
   <si>
     <t>Team Cherry</t>
-  </si>
-  <si>
-    <t>Like a Dragon: Infinite Wealth</t>
-  </si>
-  <si>
-    <t>Like a Dragon Gaiden: The Man Who Erased His Name</t>
   </si>
 </sst>
 </file>
@@ -1232,13 +1232,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A171" sqref="A171"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4446,7 +4451,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="B167" s="2">
         <v>45288</v>
@@ -4463,7 +4468,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B168" s="2">
         <v>45351</v>
@@ -4483,7 +4488,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B169" s="2">
         <v>45481</v>
@@ -4503,13 +4508,13 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B170" s="2">
         <v>45533</v>
       </c>
       <c r="C170" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D170" t="s">
         <v>206</v>
@@ -4520,7 +4525,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B171" s="2">
         <v>45556</v>
@@ -4537,13 +4542,13 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B172" s="2">
         <v>45575</v>
       </c>
       <c r="C172" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D172" t="s">
         <v>8</v>
@@ -4557,7 +4562,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="B173" s="2">
         <v>45591</v>
@@ -4574,7 +4579,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B174" s="2">
         <v>45604</v>
@@ -4591,13 +4596,13 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B175" s="2">
         <v>45613</v>
       </c>
       <c r="C175" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D175" t="s">
         <v>206</v>
@@ -4608,7 +4613,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B176" s="2">
         <v>45647</v>
@@ -4625,7 +4630,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B177" s="2">
         <v>45676</v>
@@ -4642,13 +4647,13 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B178" s="2">
         <v>45709</v>
       </c>
       <c r="C178" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D178" t="s">
         <v>206</v>
@@ -4659,7 +4664,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B179" s="2">
         <v>45725</v>
@@ -4676,13 +4681,13 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B180" s="2">
         <v>45777</v>
       </c>
       <c r="C180" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D180" t="s">
         <v>206</v>
@@ -4693,13 +4698,13 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B181" s="2">
         <v>45793</v>
       </c>
       <c r="C181" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D181" t="s">
         <v>206</v>
@@ -4710,7 +4715,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B182" s="2">
         <v>45848</v>
@@ -4727,13 +4732,13 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B183" s="2">
         <v>45899</v>
       </c>
       <c r="C183" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D183" t="s">
         <v>206</v>
@@ -4744,13 +4749,13 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B184" s="2">
         <v>45934</v>
       </c>
       <c r="C184" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D184" t="s">
         <v>206</v>

</xml_diff>